<commit_message>
platform name is not reflated in the clint_config.cfg file issue resolved
automation srcipts has been midified

bandwidth unit has been changed in the storage tab of Performance_Template.xlsx

hardware info and stress ng tool has failed for execution in results_summary file issue is fixed
</commit_message>
<xml_diff>
--- a/frontend/polls/templates/polls/Performance_Template.xlsx
+++ b/frontend/polls/templates/polls/Performance_Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="941" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="941" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="algorithm" sheetId="1" state="visible" r:id="rId2"/>
@@ -492,7 +492,7 @@
     <t>random_write</t>
   </si>
   <si>
-    <t>bytes/second</t>
+    <t>Mbytes/second</t>
   </si>
   <si>
     <t>reread</t>
@@ -1140,8 +1140,8 @@
   </sheetPr>
   <dimension ref="1:29"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -41257,13 +41257,15 @@
   </sheetPr>
   <dimension ref="A1:M36"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I39" activeCellId="0" sqref="I39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="12" min="1" style="1" width="12.004048582996"/>
+    <col collapsed="false" hidden="false" max="4" min="1" style="1" width="12.004048582996"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="16.9028340080972"/>
+    <col collapsed="false" hidden="false" max="12" min="6" style="1" width="12.004048582996"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="1" width="9.1417004048583"/>
     <col collapsed="false" hidden="false" max="15" min="14" style="0" width="9.1417004048583"/>
     <col collapsed="false" hidden="false" max="17" min="16" style="0" width="8.5748987854251"/>

</xml_diff>

<commit_message>
update sysbench parser logic.
update hardware info parser to add exception

add the logic for generating covariance for multiple iterations

platform name is not reflacted in client_config files for automation scripts

all the automation scripts are modified as updated by prashanth

bandwidth unit has been changed in storage tab of Performance_Template.xls

update target_dependency.sh file. generic version of mysql-server has been checked

update stressng_parser.py file to resolve the issue of stressng values are not being reflacted in yaml file

UDP_RR test case is not being executed by netperf tool. Because the command option for the test case is wrong in netperf_run.cfg file.
</commit_message>
<xml_diff>
--- a/frontend/polls/templates/polls/Performance_Template.xlsx
+++ b/frontend/polls/templates/polls/Performance_Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="941" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="941" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="algorithm" sheetId="1" state="visible" r:id="rId2"/>
@@ -492,7 +492,7 @@
     <t>random_write</t>
   </si>
   <si>
-    <t>bytes/second</t>
+    <t>Mbytes/second</t>
   </si>
   <si>
     <t>reread</t>
@@ -1136,11 +1136,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
+    <tabColor rgb="00FFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="1:29"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1912,6 +1913,7 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
+    <tabColor rgb="00FFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="1:53"/>
@@ -3313,6 +3315,7 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
+    <tabColor rgb="00FFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:AMI45"/>
@@ -37753,6 +37756,7 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
+    <tabColor rgb="00FFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:AMI28"/>
@@ -41253,17 +41257,20 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
+    <tabColor rgb="00FFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:M36"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G24" activeCellId="0" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="12" min="1" style="1" width="12.004048582996"/>
+    <col collapsed="false" hidden="false" max="4" min="1" style="1" width="12.004048582996"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="17.4898785425101"/>
+    <col collapsed="false" hidden="false" max="12" min="6" style="1" width="12.004048582996"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="1" width="9.1417004048583"/>
     <col collapsed="false" hidden="false" max="15" min="14" style="0" width="9.1417004048583"/>
     <col collapsed="false" hidden="false" max="17" min="16" style="0" width="8.5748987854251"/>
@@ -42197,6 +42204,7 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
+    <tabColor rgb="00FFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:M39"/>
@@ -43220,6 +43228,7 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
+    <tabColor rgb="00FFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="1:36"/>
@@ -44201,6 +44210,7 @@
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
+    <tabColor rgb="00FFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:Q16"/>

</xml_diff>

<commit_message>
Add network test cases and update naming convention in Performance_Template.xlsx file.
</commit_message>
<xml_diff>
--- a/frontend/polls/templates/polls/Performance_Template.xlsx
+++ b/frontend/polls/templates/polls/Performance_Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="941" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="970" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="algorithm" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1143" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1176" uniqueCount="289">
   <si>
     <t>Caliper Performance Tests: Algorithm</t>
   </si>
@@ -183,31 +183,31 @@
     <t>compile</t>
   </si>
   <si>
-    <t>Kernel-dev_1</t>
+    <t>kernel-dev_01</t>
   </si>
   <si>
     <t>Kilo sec</t>
   </si>
   <si>
-    <t>Kernel-dev_2</t>
+    <t>kernel-dev_02</t>
   </si>
   <si>
-    <t>Kernel-dev_4</t>
+    <t>kernel-dev_04</t>
   </si>
   <si>
-    <t>Kernel-dev_8</t>
+    <t>kernel-dev_08</t>
   </si>
   <si>
-    <t>Kernel-dev_16</t>
+    <t>kernel-dev_16</t>
   </si>
   <si>
-    <t>Kernel-dev_32</t>
+    <t>kernel-dev_32</t>
   </si>
   <si>
-    <t>Kernel-dev_64</t>
+    <t>kernel-dev_64</t>
   </si>
   <si>
-    <t>Kernel-dev_72</t>
+    <t>kernel-dev_72</t>
   </si>
   <si>
     <t>ebizzy</t>
@@ -216,16 +216,16 @@
     <t>ebizzy_no_mmap_time</t>
   </si>
   <si>
-    <t>sys_1</t>
+    <t>sys_01</t>
   </si>
   <si>
-    <t>sys_2</t>
+    <t>sys_02</t>
   </si>
   <si>
-    <t>sys_4</t>
+    <t>sys_04</t>
   </si>
   <si>
-    <t>sys_8</t>
+    <t>sys_08</t>
   </si>
   <si>
     <t>sys_16</t>
@@ -243,16 +243,16 @@
     <t>ebizzy_no_mmap_records</t>
   </si>
   <si>
-    <t>records_1</t>
+    <t>records_01</t>
   </si>
   <si>
-    <t>records_2</t>
+    <t>records_02</t>
   </si>
   <si>
-    <t>records_4</t>
+    <t>records_04</t>
   </si>
   <si>
-    <t>records_8</t>
+    <t>records_08</t>
   </si>
   <si>
     <t>records_16</t>
@@ -639,19 +639,19 @@
     <t>ctx</t>
   </si>
   <si>
-    <t>2p/64K_ctxsw</t>
+    <t>02p/0K_ctxsw</t>
   </si>
   <si>
-    <t>2p/0K_ctxsw</t>
+    <t>02p/16K_ctxsw</t>
   </si>
   <si>
-    <t>8p/64K_ctxsw</t>
+    <t>02p/64K_ctxsw</t>
   </si>
   <si>
-    <t>8p/16K_ctxsw</t>
+    <t>08p/16K_ctxsw</t>
   </si>
   <si>
-    <t>2p/16K_ctxsw</t>
+    <t>08p/64K_ctxsw</t>
   </si>
   <si>
     <t>16p/16K_ctxsw</t>
@@ -834,19 +834,52 @@
     <t>iperf</t>
   </si>
   <si>
-    <t>TCP_s5</t>
+    <t>TCP_s01_RX</t>
   </si>
   <si>
     <t>Mbytesec</t>
   </si>
   <si>
-    <t>TCP_s3</t>
+    <t>TCP_s01_TX</t>
   </si>
   <si>
-    <t>TCP_s1</t>
+    <t>TCP_s03_RX</t>
   </si>
   <si>
-    <t>TCP_s10</t>
+    <t>TCP_s03_TX</t>
+  </si>
+  <si>
+    <t>TCP_s05_RX</t>
+  </si>
+  <si>
+    <t>TCP_s05_TX</t>
+  </si>
+  <si>
+    <t>TCP_s10_RX</t>
+  </si>
+  <si>
+    <t>TCP_s10_TX</t>
+  </si>
+  <si>
+    <t>UDP_s01_TX</t>
+  </si>
+  <si>
+    <t>UDP_s03_RX</t>
+  </si>
+  <si>
+    <t>UDP_s03_TX</t>
+  </si>
+  <si>
+    <t>UDP_s05_RX</t>
+  </si>
+  <si>
+    <t>UDP_s05_TX</t>
+  </si>
+  <si>
+    <t>UDP_s10_RX</t>
+  </si>
+  <si>
+    <t>UDP_s10_TX</t>
   </si>
   <si>
     <t>local_lat</t>
@@ -1136,7 +1169,6 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <tabColor rgb="00FFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="1:29"/>
@@ -1147,14 +1179,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="5.17813765182186"/>
-    <col collapsed="false" hidden="false" max="7" min="2" style="1" width="9.81376518218623"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="11.5748987854251"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="10.4696356275304"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="11.2388663967611"/>
-    <col collapsed="false" hidden="false" max="13" min="11" style="1" width="12.4534412955466"/>
-    <col collapsed="false" hidden="false" max="1022" min="14" style="1" width="9.1417004048583"/>
-    <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="5.24696356275304"/>
+    <col collapsed="false" hidden="false" max="7" min="2" style="1" width="9.96356275303644"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="11.5708502024291"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="10.497975708502"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="11.246963562753"/>
+    <col collapsed="false" hidden="false" max="13" min="11" style="1" width="12.6396761133603"/>
+    <col collapsed="false" hidden="false" max="1022" min="14" style="1" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="36.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1913,30 +1945,29 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <tabColor rgb="00FFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="1:53"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="5.50607287449393"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="10.6923076923077"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="13.7165991902834"/>
-    <col collapsed="false" hidden="false" max="7" min="5" style="1" width="10.6923076923077"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="11.7975708502024"/>
-    <col collapsed="false" hidden="false" max="10" min="9" style="1" width="10.6923076923077"/>
-    <col collapsed="false" hidden="false" max="12" min="11" style="1" width="12.6761133603239"/>
-    <col collapsed="false" hidden="false" max="14" min="13" style="1" width="9.1417004048583"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="9.1417004048583"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="10.6923076923077"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="12.6761133603239"/>
-    <col collapsed="false" hidden="false" max="1023" min="18" style="1" width="10.6923076923077"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="10.6923076923077"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="5.57085020242915"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="10.7125506072875"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="13.7125506072874"/>
+    <col collapsed="false" hidden="false" max="7" min="5" style="1" width="10.7125506072875"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="11.7813765182186"/>
+    <col collapsed="false" hidden="false" max="10" min="9" style="1" width="10.7125506072875"/>
+    <col collapsed="false" hidden="false" max="12" min="11" style="1" width="12.8542510121458"/>
+    <col collapsed="false" hidden="false" max="14" min="13" style="1" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="10.7125506072875"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="12.8542510121458"/>
+    <col collapsed="false" hidden="false" max="1023" min="18" style="1" width="10.7125506072875"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="10.7125506072875"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="41.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3315,7 +3346,6 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <tabColor rgb="00FFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:AMI45"/>
@@ -3326,17 +3356,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="5.61943319838057"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="10.246963562753"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="1" width="10.9109311740891"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="11.5748987854251"/>
-    <col collapsed="false" hidden="false" max="12" min="6" style="1" width="10.9109311740891"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="9.1417004048583"/>
-    <col collapsed="false" hidden="false" max="15" min="14" style="0" width="9.1417004048583"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="10.9109311740891"/>
-    <col collapsed="false" hidden="false" max="18" min="17" style="0" width="10.9109311740891"/>
-    <col collapsed="false" hidden="false" max="1023" min="19" style="1" width="10.9109311740891"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="10.9109311740891"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="5.67611336032389"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="10.3886639676113"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="1" width="10.9271255060729"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="11.5708502024291"/>
+    <col collapsed="false" hidden="false" max="12" min="6" style="1" width="10.9271255060729"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="15" min="14" style="0" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="10.9271255060729"/>
+    <col collapsed="false" hidden="false" max="18" min="17" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="1023" min="19" style="1" width="10.9271255060729"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="38.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -37756,28 +37786,27 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <tabColor rgb="00FFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:AMI28"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="5.61943319838057"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="10.246963562753"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="10.9109311740891"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="25.7935222672065"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="11.5748987854251"/>
-    <col collapsed="false" hidden="false" max="13" min="6" style="1" width="10.9109311740891"/>
-    <col collapsed="false" hidden="false" max="15" min="14" style="0" width="10.9109311740891"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="10.9109311740891"/>
-    <col collapsed="false" hidden="false" max="18" min="17" style="0" width="10.9109311740891"/>
-    <col collapsed="false" hidden="false" max="1023" min="19" style="1" width="10.9109311740891"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="10.9109311740891"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="5.67611336032389"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="10.3886639676113"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="10.9271255060729"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="26.0283400809717"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="11.5708502024291"/>
+    <col collapsed="false" hidden="false" max="13" min="6" style="1" width="10.9271255060729"/>
+    <col collapsed="false" hidden="false" max="15" min="14" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="10.9271255060729"/>
+    <col collapsed="false" hidden="false" max="18" min="17" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="1023" min="19" style="1" width="10.9271255060729"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="38.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -41257,24 +41286,23 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <tabColor rgb="00FFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:M36"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G24" activeCellId="0" sqref="G24"/>
+      <selection pane="topLeft" activeCell="J23" activeCellId="0" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="4" min="1" style="1" width="12.004048582996"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="17.4898785425101"/>
-    <col collapsed="false" hidden="false" max="12" min="6" style="1" width="12.004048582996"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="9.1417004048583"/>
-    <col collapsed="false" hidden="false" max="15" min="14" style="0" width="9.1417004048583"/>
-    <col collapsed="false" hidden="false" max="17" min="16" style="0" width="8.5748987854251"/>
-    <col collapsed="false" hidden="false" max="1025" min="18" style="1" width="12.004048582996"/>
+    <col collapsed="false" hidden="false" max="4" min="1" style="1" width="12.2105263157895"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="18.080971659919"/>
+    <col collapsed="false" hidden="false" max="12" min="6" style="1" width="12.2105263157895"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="15" min="14" style="0" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="17" min="16" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="1025" min="18" style="1" width="12.2105263157895"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="42.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -42204,32 +42232,31 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <tabColor rgb="00FFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:M39"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="5.8421052631579"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="8.70445344129555"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.1336032388664"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="8.70445344129555"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="1" width="10.582995951417"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="5.89068825910931"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="8.67611336032389"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.1417004048583"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="8.67611336032389"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="1" width="10.6032388663968"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="1" width="11.4615384615385"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="10.582995951417"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="11.9028340080972"/>
-    <col collapsed="false" hidden="false" max="13" min="11" style="1" width="11.0202429149798"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="8.70445344129555"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="11.9028340080972"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="11.7975708502024"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="11.0202429149798"/>
-    <col collapsed="false" hidden="false" max="19" min="18" style="0" width="10.582995951417"/>
-    <col collapsed="false" hidden="false" max="1025" min="20" style="1" width="8.70445344129555"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="10.6032388663968"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="12.1052631578947"/>
+    <col collapsed="false" hidden="false" max="13" min="11" style="1" width="11.0323886639676"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="8.67611336032389"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="12.1052631578947"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="11.7813765182186"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="11.0323886639676"/>
+    <col collapsed="false" hidden="false" max="19" min="18" style="0" width="10.6032388663968"/>
+    <col collapsed="false" hidden="false" max="1025" min="20" style="1" width="8.67611336032389"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="38.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -43228,7 +43255,6 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <tabColor rgb="00FFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="1:36"/>
@@ -43239,22 +43265,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="5.50607287449393"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="9.25506072874494"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="17.9676113360324"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="9.25506072874494"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="1" width="9.81376518218623"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="11.5748987854251"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="9.25506072874494"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="10.8056680161943"/>
-    <col collapsed="false" hidden="false" max="13" min="11" style="1" width="11.0202429149798"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="11.0202429149798"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="10.3603238866397"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="9.25506072874494"/>
-    <col collapsed="false" hidden="false" max="18" min="17" style="1" width="9.25506072874494"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="9.25506072874494"/>
-    <col collapsed="false" hidden="false" max="1023" min="20" style="1" width="9.25506072874494"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="9.25506072874494"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="5.57085020242915"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="9.21052631578947"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.2105263157895"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="9.21052631578947"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="1" width="9.96356275303644"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="11.5708502024291"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="9.21052631578947"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="10.8178137651822"/>
+    <col collapsed="false" hidden="false" max="13" min="11" style="1" width="11.0323886639676"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="11.0323886639676"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="10.3886639676113"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="9.21052631578947"/>
+    <col collapsed="false" hidden="false" max="18" min="17" style="1" width="9.21052631578947"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="9.21052631578947"/>
+    <col collapsed="false" hidden="false" max="1023" min="20" style="1" width="9.21052631578947"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="9.21052631578947"/>
   </cols>
   <sheetData>
     <row r="1" s="19" customFormat="true" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -44210,31 +44236,30 @@
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <tabColor rgb="00FFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q16"/>
+  <dimension ref="A1:Q27"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="5.50607287449393"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="9.36842105263158"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="12.0121457489879"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="9.36842105263158"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="1" width="10.1417004048583"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="11.2388663967611"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="9.36842105263158"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="11.7975708502024"/>
-    <col collapsed="false" hidden="false" max="13" min="11" style="1" width="11.0202429149798"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="9.36842105263158"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="11.0202429149798"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="9.36842105263158"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="9.36842105263158"/>
-    <col collapsed="false" hidden="false" max="1025" min="18" style="1" width="9.36842105263158"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="5.57085020242915"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="9.31983805668016"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="12.2105263157895"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="9.31983805668016"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="1" width="10.2834008097166"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="11.246963562753"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="9.31983805668016"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="11.7813765182186"/>
+    <col collapsed="false" hidden="false" max="13" min="11" style="1" width="11.0323886639676"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="9.31983805668016"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="11.0323886639676"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="9.31983805668016"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="9.31983805668016"/>
+    <col collapsed="false" hidden="false" max="1025" min="18" style="1" width="9.31983805668016"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="33.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -44312,7 +44337,7 @@
       <c r="B3" s="7" t="s">
         <v>263</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="7" t="s">
         <v>171</v>
       </c>
       <c r="D3" s="8" t="s">
@@ -44337,7 +44362,7 @@
       <c r="B4" s="7" t="s">
         <v>263</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="7" t="s">
         <v>171</v>
       </c>
       <c r="D4" s="8" t="s">
@@ -44362,7 +44387,7 @@
       <c r="B5" s="7" t="s">
         <v>263</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="7" t="s">
         <v>171</v>
       </c>
       <c r="D5" s="8" t="s">
@@ -44387,7 +44412,7 @@
       <c r="B6" s="7" t="s">
         <v>263</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="7" t="s">
         <v>171</v>
       </c>
       <c r="D6" s="8" t="s">
@@ -44412,7 +44437,7 @@
       <c r="B7" s="7" t="s">
         <v>263</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="7" t="s">
         <v>171</v>
       </c>
       <c r="D7" s="8" t="s">
@@ -44437,7 +44462,7 @@
       <c r="B8" s="7" t="s">
         <v>269</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="7" t="s">
         <v>171</v>
       </c>
       <c r="D8" s="8" t="s">
@@ -44462,7 +44487,7 @@
       <c r="B9" s="7" t="s">
         <v>269</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="7" t="s">
         <v>171</v>
       </c>
       <c r="D9" s="8" t="s">
@@ -44487,7 +44512,7 @@
       <c r="B10" s="7" t="s">
         <v>269</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="7" t="s">
         <v>171</v>
       </c>
       <c r="D10" s="8" t="s">
@@ -44506,13 +44531,9 @@
       <c r="M10" s="8"/>
     </row>
     <row r="11" customFormat="false" ht="15.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="7" t="n">
-        <v>9</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>269</v>
-      </c>
-      <c r="C11" s="6" t="s">
+      <c r="A11" s="7"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7" t="s">
         <v>171</v>
       </c>
       <c r="D11" s="8" t="s">
@@ -44530,21 +44551,17 @@
       <c r="L11" s="8"/>
       <c r="M11" s="8"/>
     </row>
-    <row r="12" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="7" t="n">
-        <v>3</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>114</v>
-      </c>
+    <row r="12" customFormat="false" ht="15.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="7"/>
+      <c r="B12" s="7"/>
       <c r="C12" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="D12" s="8" t="s">
         <v>275</v>
       </c>
-      <c r="D12" s="8" t="s">
-        <v>249</v>
-      </c>
       <c r="E12" s="8" t="s">
-        <v>181</v>
+        <v>271</v>
       </c>
       <c r="F12" s="9"/>
       <c r="G12" s="8"/>
@@ -44555,21 +44572,17 @@
       <c r="L12" s="8"/>
       <c r="M12" s="8"/>
     </row>
-    <row r="13" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="7" t="n">
-        <v>11</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>114</v>
-      </c>
+    <row r="13" customFormat="false" ht="15.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="7"/>
+      <c r="B13" s="7"/>
       <c r="C13" s="7" t="s">
-        <v>275</v>
+        <v>171</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>245</v>
+        <v>276</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>181</v>
+        <v>271</v>
       </c>
       <c r="F13" s="9"/>
       <c r="G13" s="8"/>
@@ -44580,21 +44593,17 @@
       <c r="L13" s="8"/>
       <c r="M13" s="8"/>
     </row>
-    <row r="14" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="7" t="n">
-        <v>12</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>114</v>
-      </c>
+    <row r="14" customFormat="false" ht="15.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="7"/>
+      <c r="B14" s="7"/>
       <c r="C14" s="7" t="s">
-        <v>275</v>
+        <v>171</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>181</v>
+        <v>271</v>
       </c>
       <c r="F14" s="9"/>
       <c r="G14" s="8"/>
@@ -44605,21 +44614,17 @@
       <c r="L14" s="8"/>
       <c r="M14" s="8"/>
     </row>
-    <row r="15" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="7" t="n">
-        <v>13</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>114</v>
-      </c>
+    <row r="15" customFormat="false" ht="15.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="7"/>
+      <c r="B15" s="7"/>
       <c r="C15" s="7" t="s">
-        <v>275</v>
+        <v>171</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>181</v>
+        <v>271</v>
       </c>
       <c r="F15" s="9"/>
       <c r="G15" s="8"/>
@@ -44630,21 +44635,17 @@
       <c r="L15" s="8"/>
       <c r="M15" s="8"/>
     </row>
-    <row r="16" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="7" t="n">
-        <v>14</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>114</v>
-      </c>
+    <row r="16" customFormat="false" ht="15.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="7"/>
+      <c r="B16" s="7"/>
       <c r="C16" s="7" t="s">
-        <v>275</v>
+        <v>171</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>258</v>
+        <v>279</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>181</v>
+        <v>271</v>
       </c>
       <c r="F16" s="9"/>
       <c r="G16" s="8"/>
@@ -44655,17 +44656,272 @@
       <c r="L16" s="8"/>
       <c r="M16" s="8"/>
     </row>
+    <row r="17" customFormat="false" ht="15.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="7"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>271</v>
+      </c>
+      <c r="F17" s="9"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="8"/>
+      <c r="L17" s="8"/>
+      <c r="M17" s="8"/>
+    </row>
+    <row r="18" customFormat="false" ht="15.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="7"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>271</v>
+      </c>
+      <c r="F18" s="9"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="8"/>
+      <c r="L18" s="8"/>
+      <c r="M18" s="8"/>
+    </row>
+    <row r="19" customFormat="false" ht="15.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="7"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>271</v>
+      </c>
+      <c r="F19" s="9"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="8"/>
+      <c r="K19" s="8"/>
+      <c r="L19" s="8"/>
+      <c r="M19" s="8"/>
+    </row>
+    <row r="20" customFormat="false" ht="15.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="7"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>271</v>
+      </c>
+      <c r="F20" s="9"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="8"/>
+      <c r="K20" s="8"/>
+      <c r="L20" s="8"/>
+      <c r="M20" s="8"/>
+    </row>
+    <row r="21" customFormat="false" ht="15.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="7"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>284</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>271</v>
+      </c>
+      <c r="F21" s="9"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="8"/>
+      <c r="J21" s="8"/>
+      <c r="K21" s="8"/>
+      <c r="L21" s="8"/>
+      <c r="M21" s="8"/>
+    </row>
+    <row r="22" customFormat="false" ht="15.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="7" t="n">
+        <v>9</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>269</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>285</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>271</v>
+      </c>
+      <c r="F22" s="9"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
+      <c r="K22" s="8"/>
+      <c r="L22" s="8"/>
+      <c r="M22" s="8"/>
+    </row>
+    <row r="23" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="7" t="n">
+        <v>3</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>286</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="F23" s="9"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="8"/>
+      <c r="K23" s="8"/>
+      <c r="L23" s="8"/>
+      <c r="M23" s="8"/>
+    </row>
+    <row r="24" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="7" t="n">
+        <v>11</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>286</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="F24" s="9"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="8"/>
+      <c r="I24" s="8"/>
+      <c r="J24" s="8"/>
+      <c r="K24" s="8"/>
+      <c r="L24" s="8"/>
+      <c r="M24" s="8"/>
+    </row>
+    <row r="25" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="7" t="n">
+        <v>12</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>286</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>287</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="F25" s="9"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="8"/>
+      <c r="I25" s="8"/>
+      <c r="J25" s="8"/>
+      <c r="K25" s="8"/>
+      <c r="L25" s="8"/>
+      <c r="M25" s="8"/>
+    </row>
+    <row r="26" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="7" t="n">
+        <v>13</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>286</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>288</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="F26" s="9"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="8"/>
+      <c r="I26" s="8"/>
+      <c r="J26" s="8"/>
+      <c r="K26" s="8"/>
+      <c r="L26" s="8"/>
+      <c r="M26" s="8"/>
+    </row>
+    <row r="27" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A27" s="7" t="n">
+        <v>14</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>286</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>258</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="F27" s="9"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="8"/>
+      <c r="I27" s="8"/>
+      <c r="J27" s="8"/>
+      <c r="K27" s="8"/>
+      <c r="L27" s="8"/>
+      <c r="M27" s="8"/>
+    </row>
   </sheetData>
   <mergeCells count="9">
     <mergeCell ref="A1:M1"/>
     <mergeCell ref="A3:A7"/>
     <mergeCell ref="B3:B7"/>
-    <mergeCell ref="C3:C11"/>
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="B8:B11"/>
-    <mergeCell ref="A12:A16"/>
-    <mergeCell ref="B12:B16"/>
-    <mergeCell ref="C12:C16"/>
+    <mergeCell ref="C3:C22"/>
+    <mergeCell ref="A8:A22"/>
+    <mergeCell ref="B8:B22"/>
+    <mergeCell ref="A23:A27"/>
+    <mergeCell ref="B23:B27"/>
+    <mergeCell ref="C23:C27"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>